<commit_message>
Update test case 20160331 - 002
</commit_message>
<xml_diff>
--- a/20160331 - 002/running_logs/logs.xlsx
+++ b/20160331 - 002/running_logs/logs.xlsx
@@ -43,10 +43,10 @@
     <t>Template Filter</t>
   </si>
   <si>
-    <t>20160401_013014</t>
-  </si>
-  <si>
-    <t>remove multiple spaces, convert unicode to ascii, convert to lower, trim "space" and ","</t>
+    <t>20160403_213812</t>
+  </si>
+  <si>
+    <t>trim "space" and ",", convert to lower, remove multiple spaces, convert unicode to ascii</t>
   </si>
   <si>
     <t>5 features: #ascii/(#ascii+#digit+#punctuation), #max_digit_skip_0_1, #(, #+, #/</t>
@@ -61,19 +61,19 @@
     <t xml:space="preserve">0 filters: </t>
   </si>
   <si>
-    <t>20160401_013158</t>
-  </si>
-  <si>
-    <t>20160401_013341</t>
-  </si>
-  <si>
-    <t>20160401_013538</t>
-  </si>
-  <si>
-    <t>20160401_013736</t>
-  </si>
-  <si>
-    <t>20160401_015220</t>
+    <t>20160403_213948</t>
+  </si>
+  <si>
+    <t>20160403_214125</t>
+  </si>
+  <si>
+    <t>20160403_214311</t>
+  </si>
+  <si>
+    <t>20160403_214559</t>
+  </si>
+  <si>
+    <t>20160403_220446</t>
   </si>
   <si>
     <t>trim "space" and ",", convert unicode to ascii, convert to lower, remove multiple spaces</t>
@@ -82,16 +82,16 @@
     <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 300</t>
   </si>
   <si>
-    <t>20160401_015945</t>
-  </si>
-  <si>
-    <t>20160401_020956</t>
-  </si>
-  <si>
-    <t>20160401_021921</t>
-  </si>
-  <si>
-    <t>20160401_022928</t>
+    <t>20160403_225315</t>
+  </si>
+  <si>
+    <t>20160403_230041</t>
+  </si>
+  <si>
+    <t>20160403_230721</t>
+  </si>
+  <si>
+    <t>20160403_231406</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>104.157</v>
+        <v>95.164</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -478,7 +478,7 @@
         <v>13</v>
       </c>
       <c r="G2">
-        <v>0.954666666666667</v>
+        <v>0.957333333333333</v>
       </c>
       <c r="H2">
         <v>0.996699669966997</v>
@@ -487,7 +487,7 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <v>0.336734693877551</v>
+        <v>0.214285714285714</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -495,7 +495,7 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>102.523</v>
+        <v>97.81</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -510,7 +510,7 @@
         <v>13</v>
       </c>
       <c r="G3">
-        <v>0.96</v>
+        <v>0.964</v>
       </c>
       <c r="H3">
         <v>0.996699669966997</v>
@@ -519,7 +519,7 @@
         <v>14</v>
       </c>
       <c r="J3">
-        <v>0.326530612244898</v>
+        <v>0.214285714285714</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -527,7 +527,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>117.303</v>
+        <v>105.718</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -542,7 +542,7 @@
         <v>13</v>
       </c>
       <c r="G4">
-        <v>0.962</v>
+        <v>0.965333333333333</v>
       </c>
       <c r="H4">
         <v>0.996699669966997</v>
@@ -551,7 +551,7 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <v>0.336734693877551</v>
+        <v>0.214285714285714</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -559,7 +559,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>117.73</v>
+        <v>167.816</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -574,7 +574,7 @@
         <v>13</v>
       </c>
       <c r="G5">
-        <v>0.959333333333333</v>
+        <v>0.963333333333333</v>
       </c>
       <c r="H5">
         <v>0.996699669966997</v>
@@ -583,7 +583,7 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <v>0.316326530612245</v>
+        <v>0.214285714285714</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -591,7 +591,7 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>118.099</v>
+        <v>179.891</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -606,7 +606,7 @@
         <v>13</v>
       </c>
       <c r="G6">
-        <v>0.96</v>
+        <v>0.965333333333333</v>
       </c>
       <c r="H6">
         <v>0.996699669966997</v>
@@ -615,7 +615,7 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <v>0.316326530612245</v>
+        <v>0.214285714285714</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -623,7 +623,7 @@
         <v>19</v>
       </c>
       <c r="B7">
-        <v>445.096</v>
+        <v>2908.5</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -638,7 +638,7 @@
         <v>21</v>
       </c>
       <c r="G7">
-        <v>0.951333333333333</v>
+        <v>0.964</v>
       </c>
       <c r="H7">
         <v>0.996699669966997</v>
@@ -647,7 +647,7 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <v>0.357142857142857</v>
+        <v>0.214285714285714</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -655,7 +655,7 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>610.582</v>
+        <v>446.458</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -670,7 +670,7 @@
         <v>21</v>
       </c>
       <c r="G8">
-        <v>0.957333333333333</v>
+        <v>0.956</v>
       </c>
       <c r="H8">
         <v>0.996699669966997</v>
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <v>0.326530612244898</v>
+        <v>0.214285714285714</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -687,7 +687,7 @@
         <v>23</v>
       </c>
       <c r="B9">
-        <v>564.939</v>
+        <v>399.533</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -702,7 +702,7 @@
         <v>21</v>
       </c>
       <c r="G9">
-        <v>0.958</v>
+        <v>0.954666666666667</v>
       </c>
       <c r="H9">
         <v>0.996699669966997</v>
@@ -711,7 +711,7 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <v>0.326530612244898</v>
+        <v>0.224489795918367</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -719,7 +719,7 @@
         <v>24</v>
       </c>
       <c r="B10">
-        <v>607.277</v>
+        <v>405.343</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -734,7 +734,7 @@
         <v>21</v>
       </c>
       <c r="G10">
-        <v>0.958666666666667</v>
+        <v>0.959333333333333</v>
       </c>
       <c r="H10">
         <v>0.996699669966997</v>
@@ -743,7 +743,7 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <v>0.346938775510204</v>
+        <v>0.224489795918367</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -751,7 +751,7 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>710.739</v>
+        <v>433.539</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -766,7 +766,7 @@
         <v>21</v>
       </c>
       <c r="G11">
-        <v>0.960666666666667</v>
+        <v>0.962666666666667</v>
       </c>
       <c r="H11">
         <v>0.996699669966997</v>
@@ -775,7 +775,7 @@
         <v>14</v>
       </c>
       <c r="J11">
-        <v>0.336734693877551</v>
+        <v>0.204081632653061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>